<commit_message>
added subsetByCoord, compareByCoord and plotCompareByCoord functions
</commit_message>
<xml_diff>
--- a/inst/extdata/snoRNAdb.xlsx
+++ b/inst/extdata/snoRNAdb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\RNAmodR\literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\github\RNAmodR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC676F55-52E7-4B24-8ABF-E6DB6DB1A4E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AADA015-86AF-4460-8A93-03ECEEDA3758}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{C7F77C52-184F-48D6-8341-1B5AE4F1C940}"/>
   </bookViews>
@@ -699,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -715,7 +715,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1013,11 +1013,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBE3D91-ABC9-4AA9-9377-9C6A56725C28}">
   <dimension ref="A1:K236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -3837,7 +3837,7 @@
         <v>1869</v>
       </c>
       <c r="D81" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E81" t="s">
         <v>4</v>

</xml_diff>